<commit_message>
Piechart file and dataframe upload
</commit_message>
<xml_diff>
--- a/all_roi_df.xlsx
+++ b/all_roi_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhessa/flybrain-clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0422AB0-DBB4-E94F-BFFF-48498F8E55AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED6023C-D1EA-174E-A88C-64F0B54381E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15820" yWindow="2860" windowWidth="28040" windowHeight="17440" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
+    <workbookView xWindow="31400" yWindow="2860" windowWidth="12460" windowHeight="17320" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="236">
   <si>
     <t>Super</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t>L4</t>
+  </si>
+  <si>
+    <t>NotPrimary</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3DED42-EFA8-9A4A-A075-831208CC5CF7}">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:D231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="A231" sqref="A231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2070,17 +2073,17 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C183" t="s">
+      <c r="B183" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C184" t="s">
+      <c r="B184" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C185" t="s">
+      <c r="B185" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2090,32 +2093,32 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C187" t="s">
+      <c r="B187" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C188" t="s">
+      <c r="B188" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C189" t="s">
+      <c r="B189" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C190" t="s">
+      <c r="B190" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C191" t="s">
+      <c r="B191" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C192" t="s">
+      <c r="B192" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2307,6 +2310,11 @@
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update version number in piechart_ovi.ipynb
</commit_message>
<xml_diff>
--- a/all_roi_df.xlsx
+++ b/all_roi_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhessa/flybrain-clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED6023C-D1EA-174E-A88C-64F0B54381E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0902B285-63C5-7849-918D-CD7989E06A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31400" yWindow="2860" windowWidth="12460" windowHeight="17320" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
+    <workbookView xWindow="21280" yWindow="1920" windowWidth="22720" windowHeight="21360" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="244">
   <si>
     <t>Super</t>
   </si>
@@ -754,6 +754,30 @@
   </si>
   <si>
     <t>NotPrimary</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>LX</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>SNP</t>
+  </si>
+  <si>
+    <t>VLNP</t>
+  </si>
+  <si>
+    <t>L1</t>
   </si>
 </sst>
 </file>
@@ -846,9 +870,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -886,7 +910,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -992,7 +1016,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1134,7 +1158,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1142,1178 +1166,1235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3DED42-EFA8-9A4A-A075-831208CC5CF7}">
-  <dimension ref="A1:D231"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="A231" sqref="A231"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
+      <c r="B82" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C92" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C94" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C95" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C96" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C101" t="s">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C102" t="s">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
+    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
+    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C104" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
+    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D106" t="s">
+    <row r="106" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E106" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D107" t="s">
+    <row r="107" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E107" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D108" t="s">
+    <row r="108" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E108" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C109" t="s">
+    <row r="109" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D110" t="s">
+    <row r="110" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E110" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D111" t="s">
+    <row r="111" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E111" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D112" t="s">
+    <row r="112" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E112" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C114" t="s">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C115" t="s">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C116" t="s">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C117" t="s">
+    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
+    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C120" t="s">
+    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C121" t="s">
+    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
+    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C123" t="s">
+    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C124" t="s">
+    <row r="124" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C125" t="s">
+    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C126" t="s">
+    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C127" t="s">
+    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C128" t="s">
+    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C129" t="s">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C130" t="s">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C131" t="s">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B132" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B133" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B134" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B135" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B136" t="s">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C136" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B137" t="s">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C137" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B138" t="s">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C138" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C139" t="s">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C140" t="s">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B141" t="s">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C141" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C142" t="s">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C143" t="s">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C144" s="1" t="s">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D144" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B145" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C145" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B146" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C146" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B147" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C147" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B148" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C148" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B149" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>238</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>239</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B152" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C152" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B153" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C153" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>239</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B155" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C155" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B156" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C156" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C157" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C158" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D158" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>240</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B160" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C160" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C161" t="s">
+    <row r="161" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D161" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C162" t="s">
+    <row r="162" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D162" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C163" t="s">
+    <row r="163" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D163" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D164" t="s">
+    <row r="164" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E164" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
+    <row r="165" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E165" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D166" t="s">
+    <row r="166" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E166" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C167" t="s">
+    <row r="167" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D167" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D168" t="s">
+    <row r="168" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E168" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D169" t="s">
+    <row r="169" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E169" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D170" t="s">
+    <row r="170" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E170" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C171" t="s">
+    <row r="171" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D171" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D172" t="s">
+    <row r="172" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E172" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D173" t="s">
+    <row r="173" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E173" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C174" t="s">
+    <row r="174" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D174" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D175" t="s">
+    <row r="175" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E175" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D176" t="s">
+    <row r="176" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E176" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C177" t="s">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D177" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D178" t="s">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E178" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D179" t="s">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D180" t="s">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E180" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D181" t="s">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E181" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D182" t="s">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E182" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B183" t="s">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C183" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B184" t="s">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C184" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B185" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C185" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A186" s="1" t="s">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>240</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B187" t="s">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C187" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B188" t="s">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C188" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B189" t="s">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C189" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B190" t="s">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C190" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B191" t="s">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C191" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B192" t="s">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C192" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="1" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>237</v>
+      </c>
+      <c r="B193" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B194" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B195" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C195" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B196" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C196" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B197" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C197" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="1" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B199" t="s">
+      <c r="B198" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C199" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B200" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C200" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B201" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C201" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B202" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C202" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C203" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D203" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C204" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D204" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205" s="1" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" s="1" t="s">
+      <c r="B205" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>241</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B207" t="s">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C207" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B208" t="s">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C208" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="1" t="s">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>241</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B210" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C210" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B211" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C211" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B212" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C212" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="1" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>242</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B214" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C214" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B215" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C215" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B216" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C216" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B217" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C217" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B218" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C218" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="1" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B220" t="s">
+      <c r="B219" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C220" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B221" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C221" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B222" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C222" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B223" t="s">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C223" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B224" t="s">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C224" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B225" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C225" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B226" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C226" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B227" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B228" t="s">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>236</v>
+      </c>
+      <c r="B229" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>236</v>
+      </c>
+      <c r="B230" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B231" s="1" t="s">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementing changes requested during meeting
</commit_message>
<xml_diff>
--- a/all_roi_df.xlsx
+++ b/all_roi_df.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhessa/flybrain-clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0902B285-63C5-7849-918D-CD7989E06A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0A2CA3-C660-0E45-B1F6-3367190EB05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21280" yWindow="1920" windowWidth="22720" windowHeight="21360" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
+    <workbookView xWindow="15620" yWindow="2080" windowWidth="22500" windowHeight="22020" xr2:uid="{218BD2C8-C60C-A140-AB23-F2F96D445C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="262">
   <si>
     <t>Super</t>
   </si>
@@ -778,6 +778,60 @@
   </si>
   <si>
     <t>L1</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>teal</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>tan</t>
+  </si>
+  <si>
+    <t>orchid</t>
+  </si>
+  <si>
+    <t>seagreen</t>
+  </si>
+  <si>
+    <t>cadetblue</t>
+  </si>
+  <si>
+    <t>navy</t>
+  </si>
+  <si>
+    <t>blueviolet</t>
+  </si>
+  <si>
+    <t>firebrick</t>
+  </si>
+  <si>
+    <t>royalblue</t>
+  </si>
+  <si>
+    <t>rosybrown</t>
+  </si>
+  <si>
+    <t>lightcoral</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3DED42-EFA8-9A4A-A075-831208CC5CF7}">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,7 +1231,7 @@
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1193,164 +1247,173 @@
       <c r="E1" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>236</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>236</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>45</v>
       </c>
@@ -1595,88 +1658,94 @@
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>237</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F81" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>6</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
         <v>134</v>
       </c>
@@ -1841,174 +1910,210 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D129" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D130" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D131" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B132" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F132" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>8</v>
+      </c>
       <c r="B133" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F133" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>9</v>
+      </c>
       <c r="B134" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F134" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>10</v>
+      </c>
       <c r="B135" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F135" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C136" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C137" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C138" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D139" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D140" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C141" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D142" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D143" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D144" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>238</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F150" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>239</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F151" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>239</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F154" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D157" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D158" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>240</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F159" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C160" t="s">
         <v>155</v>
       </c>
@@ -2093,309 +2198,345 @@
         <v>220</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D177" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E178" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E179" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E180" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E181" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E182" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C183" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C184" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C185" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>240</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C187" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C188" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C189" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C190" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C191" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C192" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>237</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F193" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C194" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C195" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C196" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C197" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>18</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F198" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C199" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C200" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C201" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C202" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D203" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D204" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>19</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F205" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>241</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F206" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C207" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C208" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>241</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F209" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C210" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C211" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C212" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>242</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F213" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C214" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C215" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C216" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C217" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C218" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>23</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F219" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C220" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C221" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C222" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C223" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C224" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C225" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C226" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C227" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C228" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>236</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F229" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>236</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F230" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="B231" s="1" t="s">
         <v>235</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>